<commit_message>
Se corrigen errores en el ordenamiento
</commit_message>
<xml_diff>
--- a/Datos_Paper.xlsx
+++ b/Datos_Paper.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10908"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Nati/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Desktop\genetic\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0B8734D3-1B2F-8644-A1A9-F156F0A55682}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="680" yWindow="1000" windowWidth="27540" windowHeight="14720" xr2:uid="{1D19DB78-D6B7-48B8-9869-52530DFAB772}"/>
+    <workbookView xWindow="675" yWindow="1005" windowWidth="27540" windowHeight="14715"/>
   </bookViews>
   <sheets>
     <sheet name="Solo Valores" sheetId="3" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -495,7 +494,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="0.0"/>
@@ -668,7 +667,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>25</xdr:col>
-      <xdr:colOff>807568</xdr:colOff>
+      <xdr:colOff>721843</xdr:colOff>
       <xdr:row>31</xdr:row>
       <xdr:rowOff>35985</xdr:rowOff>
     </xdr:to>
@@ -677,7 +676,7 @@
         <xdr:cNvPr id="15" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0DE8CA3D-BC96-4636-B01A-BAAC1F9AF2B8}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{0DE8CA3D-BC96-4636-B01A-BAAC1F9AF2B8}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1002,26 +1001,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09A8AD36-2937-408D-830E-7BF48E7DA86B}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:P62"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="O23" sqref="O23"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="5" width="11.5" style="1"/>
-    <col min="8" max="8" width="11.33203125" customWidth="1"/>
-    <col min="9" max="9" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.5" customWidth="1"/>
-    <col min="14" max="14" width="10.83203125" customWidth="1"/>
+    <col min="2" max="5" width="11.42578125" style="1"/>
+    <col min="8" max="8" width="11.28515625" customWidth="1"/>
+    <col min="9" max="9" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.42578125" customWidth="1"/>
+    <col min="14" max="14" width="10.85546875" customWidth="1"/>
     <col min="15" max="15" width="17" customWidth="1"/>
-    <col min="17" max="17" width="27.6640625" customWidth="1"/>
+    <col min="17" max="17" width="27.7109375" customWidth="1"/>
     <col min="18" max="18" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
         <v>149</v>
       </c>
@@ -1056,7 +1055,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="3" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B3" s="6" t="s">
         <v>0</v>
       </c>
@@ -1093,7 +1092,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="4" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B4" s="6" t="s">
         <v>1</v>
       </c>
@@ -1128,7 +1127,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B5" s="6" t="s">
         <v>2</v>
       </c>
@@ -1166,7 +1165,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="6" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B6" s="6" t="s">
         <v>3</v>
       </c>
@@ -1204,7 +1203,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="7" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B7" s="6" t="s">
         <v>4</v>
       </c>
@@ -1239,7 +1238,7 @@
         <v>16.8</v>
       </c>
     </row>
-    <row r="8" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B8" s="6" t="s">
         <v>5</v>
       </c>
@@ -1247,7 +1246,7 @@
         <v>2.8409582811219183</v>
       </c>
       <c r="D8" s="6">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="E8" s="6">
         <v>203</v>
@@ -1274,7 +1273,7 @@
         <v>25.6</v>
       </c>
     </row>
-    <row r="9" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B9" s="6" t="s">
         <v>6</v>
       </c>
@@ -1309,7 +1308,7 @@
         <v>34.4</v>
       </c>
     </row>
-    <row r="10" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B10" s="6" t="s">
         <v>7</v>
       </c>
@@ -1348,7 +1347,7 @@
       </c>
       <c r="P10" s="9"/>
     </row>
-    <row r="11" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B11" s="6" t="s">
         <v>8</v>
       </c>
@@ -1389,7 +1388,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="12" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B12" s="6" t="s">
         <v>9</v>
       </c>
@@ -1427,7 +1426,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="13" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B13" s="6" t="s">
         <v>10</v>
       </c>
@@ -1466,7 +1465,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="14" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B14" s="6" t="s">
         <v>11</v>
       </c>
@@ -1499,7 +1498,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B15" s="6" t="s">
         <v>12</v>
       </c>
@@ -1513,7 +1512,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="16" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B16" s="6" t="s">
         <v>13</v>
       </c>
@@ -1527,7 +1526,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="17" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B17" s="6" t="s">
         <v>14</v>
       </c>
@@ -1541,7 +1540,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="18" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B18" s="6" t="s">
         <v>15</v>
       </c>
@@ -1579,7 +1578,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="19" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B19" s="6" t="s">
         <v>16</v>
       </c>
@@ -1621,7 +1620,7 @@
         <v>107.46666666666667</v>
       </c>
     </row>
-    <row r="20" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B20" s="6" t="s">
         <v>17</v>
       </c>
@@ -1663,7 +1662,7 @@
         <v>122.13333333333333</v>
       </c>
     </row>
-    <row r="21" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B21" s="6" t="s">
         <v>18</v>
       </c>
@@ -1705,7 +1704,7 @@
         <v>136.80000000000001</v>
       </c>
     </row>
-    <row r="22" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B22" s="6" t="s">
         <v>19</v>
       </c>
@@ -1747,7 +1746,7 @@
         <v>116.26666666666667</v>
       </c>
     </row>
-    <row r="23" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B23" s="6" t="s">
         <v>20</v>
       </c>
@@ -1789,7 +1788,7 @@
         <v>130.93333333333334</v>
       </c>
     </row>
-    <row r="24" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B24" s="6" t="s">
         <v>21</v>
       </c>
@@ -1831,7 +1830,7 @@
         <v>145.6</v>
       </c>
     </row>
-    <row r="25" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B25" s="6" t="s">
         <v>22</v>
       </c>
@@ -1873,7 +1872,7 @@
         <v>125.06666666666668</v>
       </c>
     </row>
-    <row r="26" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B26" s="6" t="s">
         <v>23</v>
       </c>
@@ -1915,7 +1914,7 @@
         <v>139.73333333333335</v>
       </c>
     </row>
-    <row r="27" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B27" s="6" t="s">
         <v>24</v>
       </c>
@@ -1957,7 +1956,7 @@
         <v>154.4</v>
       </c>
     </row>
-    <row r="28" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B28" s="6" t="s">
         <v>25</v>
       </c>
@@ -1999,7 +1998,7 @@
         <v>133.86666666666665</v>
       </c>
     </row>
-    <row r="29" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B29" s="6" t="s">
         <v>26</v>
       </c>
@@ -2041,7 +2040,7 @@
         <v>148.53333333333333</v>
       </c>
     </row>
-    <row r="30" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B30" s="6" t="s">
         <v>27</v>
       </c>
@@ -2083,7 +2082,7 @@
         <v>163.19999999999999</v>
       </c>
     </row>
-    <row r="31" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B31" s="6" t="s">
         <v>28</v>
       </c>
@@ -2125,7 +2124,7 @@
         <v>142.66666666666666</v>
       </c>
     </row>
-    <row r="32" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B32" s="6" t="s">
         <v>29</v>
       </c>
@@ -2167,7 +2166,7 @@
         <v>157.33333333333334</v>
       </c>
     </row>
-    <row r="33" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B33" s="6" t="s">
         <v>30</v>
       </c>
@@ -2209,7 +2208,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="34" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B34" s="6" t="s">
         <v>31</v>
       </c>
@@ -2223,7 +2222,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="35" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B35" s="6" t="s">
         <v>32</v>
       </c>
@@ -2237,7 +2236,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="36" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B36" s="6" t="s">
         <v>33</v>
       </c>
@@ -2251,7 +2250,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="37" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B37" s="6" t="s">
         <v>34</v>
       </c>
@@ -2265,7 +2264,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="38" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B38" s="6" t="s">
         <v>35</v>
       </c>
@@ -2279,7 +2278,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="39" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B39" s="6" t="s">
         <v>36</v>
       </c>
@@ -2293,7 +2292,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="40" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B40" s="6" t="s">
         <v>37</v>
       </c>
@@ -2307,7 +2306,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="41" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B41" s="6" t="s">
         <v>38</v>
       </c>
@@ -2321,7 +2320,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="42" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B42" s="6" t="s">
         <v>39</v>
       </c>
@@ -2335,7 +2334,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="43" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B43" s="6" t="s">
         <v>40</v>
       </c>
@@ -2349,7 +2348,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="44" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B44" s="6" t="s">
         <v>41</v>
       </c>
@@ -2363,7 +2362,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="45" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B45" s="6" t="s">
         <v>42</v>
       </c>
@@ -2377,7 +2376,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="46" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="46" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B46" s="6" t="s">
         <v>43</v>
       </c>
@@ -2391,7 +2390,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="47" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="47" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B47" s="6" t="s">
         <v>44</v>
       </c>
@@ -2405,7 +2404,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="48" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="48" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B48" s="6" t="s">
         <v>45</v>
       </c>
@@ -2419,7 +2418,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="49" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="49" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B49" s="6" t="s">
         <v>46</v>
       </c>
@@ -2433,7 +2432,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="50" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="50" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B50" s="6" t="s">
         <v>47</v>
       </c>
@@ -2447,7 +2446,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="51" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="51" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B51" s="6" t="s">
         <v>48</v>
       </c>
@@ -2461,7 +2460,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="52" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="52" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B52" s="6" t="s">
         <v>49</v>
       </c>
@@ -2475,7 +2474,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="53" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="53" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B53" s="6" t="s">
         <v>51</v>
       </c>
@@ -2489,7 +2488,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="54" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="54" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B54" s="6" t="s">
         <v>52</v>
       </c>
@@ -2503,7 +2502,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="55" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="55" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B55" s="6" t="s">
         <v>53</v>
       </c>
@@ -2517,7 +2516,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="56" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="56" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B56" s="6" t="s">
         <v>54</v>
       </c>
@@ -2531,7 +2530,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="57" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="57" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B57" s="6" t="s">
         <v>55</v>
       </c>
@@ -2545,7 +2544,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="58" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="58" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B58" s="6" t="s">
         <v>56</v>
       </c>
@@ -2559,7 +2558,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="59" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="59" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B59" s="6" t="s">
         <v>57</v>
       </c>
@@ -2573,7 +2572,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="60" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="60" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B60" s="6" t="s">
         <v>58</v>
       </c>
@@ -2587,7 +2586,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="61" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="61" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B61" s="6" t="s">
         <v>59</v>
       </c>
@@ -2601,7 +2600,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="62" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="62" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B62" s="6" t="s">
         <v>60</v>
       </c>

</xml_diff>